<commit_message>
valuation of indrayani mai ghar byabasthapan, pashikel paati samrakxan, kurthali chyanepaakha
</commit_message>
<xml_diff>
--- a/ofc/estimates/new track bheterinary ukhutaar sadak/estimate_anjan.xlsx
+++ b/ofc/estimates/new track bheterinary ukhutaar sadak/estimate_anjan.xlsx
@@ -553,24 +553,6 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -584,6 +566,39 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,21 +618,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1198,113 +1198,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
     </row>
     <row r="2" spans="1:30" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
     </row>
     <row r="3" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
     </row>
     <row r="5" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
     </row>
     <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1582,11 +1582,11 @@
       <c r="B18" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="74">
+      <c r="C18" s="68">
         <f>J16</f>
         <v>52047.44</v>
       </c>
-      <c r="D18" s="74"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="51"/>
       <c r="F18" s="50"/>
       <c r="G18" s="51"/>
@@ -1600,10 +1600,10 @@
       <c r="B19" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="77">
+      <c r="C19" s="71">
         <v>40000</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="67"/>
       <c r="F19" s="48"/>
       <c r="G19" s="47"/>
@@ -1617,11 +1617,11 @@
       <c r="B20" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="78">
+      <c r="C20" s="72">
         <f>C19-C22-C23</f>
         <v>38000</v>
       </c>
-      <c r="D20" s="78"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="39">
         <f>C20/C18*100</f>
         <v>73.010315204743975</v>
@@ -1638,11 +1638,11 @@
       <c r="B21" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="74">
+      <c r="C21" s="68">
         <f>C18-C20</f>
         <v>14047.440000000002</v>
       </c>
-      <c r="D21" s="74"/>
+      <c r="D21" s="68"/>
       <c r="E21" s="39">
         <f>100-E20</f>
         <v>26.989684795256025</v>
@@ -1659,11 +1659,11 @@
       <c r="B22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="74">
+      <c r="C22" s="68">
         <f>C19*0.03</f>
         <v>1200</v>
       </c>
-      <c r="D22" s="74"/>
+      <c r="D22" s="68"/>
       <c r="E22" s="39">
         <v>3</v>
       </c>
@@ -1679,11 +1679,11 @@
       <c r="B23" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="74">
+      <c r="C23" s="68">
         <f>C19*0.02</f>
         <v>800</v>
       </c>
-      <c r="D23" s="74"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="39">
         <v>2</v>
       </c>
@@ -1763,6 +1763,13 @@
     <row r="78" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="A7:F7"/>
@@ -1771,13 +1778,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -1814,90 +1814,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="90" t="s">
+      <c r="A5" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
-      <c r="K5" s="90"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="86">
+      <c r="C6" s="79">
         <f>F18</f>
         <v>52047.44</v>
       </c>
-      <c r="D6" s="87"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1905,11 +1905,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="86">
+      <c r="J6" s="79">
         <f>I18</f>
         <v>45495.768891083135</v>
       </c>
-      <c r="K6" s="87"/>
+      <c r="K6" s="80"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -1918,77 +1918,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="I7" s="82" t="s">
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="I7" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="e">
+      <c r="A8" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="I8" s="83" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="I8" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="e">
+      <c r="A9" s="89" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="I9" s="83" t="s">
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="I9" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="85" t="s">
+      <c r="D11" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="85"/>
-      <c r="F11" s="85"/>
-      <c r="G11" s="85" t="s">
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="85"/>
-      <c r="I11" s="85"/>
-      <c r="J11" s="79" t="s">
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="80" t="s">
+      <c r="K11" s="85" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="79"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2007,8 +2007,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="79"/>
-      <c r="K12" s="80"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="85"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
@@ -2170,13 +2170,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2190,6 +2183,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2208,7 +2208,7 @@
   <dimension ref="A1:U94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,113 +2226,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
     </row>
     <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
     </row>
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
     </row>
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -2416,7 +2416,7 @@
         <v>0.82499999999999996</v>
       </c>
       <c r="G10" s="39">
-        <f t="shared" ref="G10:G31" si="0">PRODUCT(C10:F10)</f>
+        <f>PRODUCT(C10:F10)</f>
         <v>12.993749999999999</v>
       </c>
       <c r="H10" s="40"/>
@@ -2446,19 +2446,19 @@
         <v>0.5</v>
       </c>
       <c r="D11" s="38">
-        <f t="shared" ref="D11:D30" si="1">M11</f>
+        <f t="shared" ref="D11:D30" si="0">M11</f>
         <v>7</v>
       </c>
       <c r="E11" s="38">
-        <f t="shared" ref="E11:E30" si="2">(N10+N11)/2</f>
+        <f t="shared" ref="E11:E30" si="1">(N10+N11)/2</f>
         <v>5.5</v>
       </c>
       <c r="F11" s="38">
-        <f t="shared" ref="F11:F30" si="3">(O10+O11)/2</f>
+        <f t="shared" ref="F11:F30" si="2">(O10+O11)/2</f>
         <v>1.85</v>
       </c>
       <c r="G11" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G11:G31" si="3">PRODUCT(C11:F11)</f>
         <v>35.612500000000004</v>
       </c>
       <c r="H11" s="40"/>
@@ -2488,19 +2488,19 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E12" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E12" s="38">
+        <v>4.8287107589149647</v>
+      </c>
+      <c r="F12" s="38">
         <f t="shared" si="2"/>
-        <v>4.8287107589149647</v>
-      </c>
-      <c r="F12" s="38">
+        <v>1.85</v>
+      </c>
+      <c r="G12" s="39">
         <f t="shared" si="3"/>
-        <v>1.85</v>
-      </c>
-      <c r="G12" s="39">
-        <f t="shared" si="0"/>
         <v>31.265902163974395</v>
       </c>
       <c r="H12" s="40"/>
@@ -2531,19 +2531,19 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E13" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E13" s="38">
+        <v>3.6574215178299299</v>
+      </c>
+      <c r="F13" s="38">
         <f t="shared" si="2"/>
-        <v>3.6574215178299299</v>
-      </c>
-      <c r="F13" s="38">
+        <v>1.5</v>
+      </c>
+      <c r="G13" s="39">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="G13" s="39">
-        <f t="shared" si="0"/>
         <v>19.201462968607132</v>
       </c>
       <c r="H13" s="40"/>
@@ -2574,19 +2574,19 @@
         <v>0.5</v>
       </c>
       <c r="D14" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E14" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E14" s="38">
+        <v>4.1145992075586708</v>
+      </c>
+      <c r="F14" s="38">
         <f t="shared" si="2"/>
-        <v>4.1145992075586708</v>
-      </c>
-      <c r="F14" s="38">
+        <v>2</v>
+      </c>
+      <c r="G14" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G14" s="39">
-        <f t="shared" si="0"/>
         <v>28.802194452910697</v>
       </c>
       <c r="H14" s="40"/>
@@ -2617,19 +2617,19 @@
         <v>0.5</v>
       </c>
       <c r="D15" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E15" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E15" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F15" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F15" s="38">
+        <v>2.25</v>
+      </c>
+      <c r="G15" s="39">
         <f t="shared" si="3"/>
-        <v>2.25</v>
-      </c>
-      <c r="G15" s="39">
-        <f t="shared" si="0"/>
         <v>36.002743066138372</v>
       </c>
       <c r="H15" s="40"/>
@@ -2660,19 +2660,19 @@
         <v>0.5</v>
       </c>
       <c r="D16" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E16" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E16" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F16" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F16" s="38">
+        <v>2</v>
+      </c>
+      <c r="G16" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G16" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H16" s="40"/>
@@ -2703,19 +2703,19 @@
         <v>0.5</v>
       </c>
       <c r="D17" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E17" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E17" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F17" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F17" s="38">
+        <v>2</v>
+      </c>
+      <c r="G17" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G17" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H17" s="40"/>
@@ -2746,19 +2746,19 @@
         <v>0.5</v>
       </c>
       <c r="D18" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E18" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E18" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F18" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F18" s="38">
+        <v>2</v>
+      </c>
+      <c r="G18" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G18" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H18" s="40"/>
@@ -2789,19 +2789,19 @@
         <v>0.5</v>
       </c>
       <c r="D19" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E19" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E19" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F19" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F19" s="38">
+        <v>2</v>
+      </c>
+      <c r="G19" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G19" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H19" s="40"/>
@@ -2832,19 +2832,19 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E20" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E20" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F20" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F20" s="38">
+        <v>2</v>
+      </c>
+      <c r="G20" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G20" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H20" s="40"/>
@@ -2875,19 +2875,19 @@
         <v>0.5</v>
       </c>
       <c r="D21" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E21" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E21" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F21" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F21" s="38">
+        <v>2</v>
+      </c>
+      <c r="G21" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G21" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H21" s="40"/>
@@ -2918,19 +2918,19 @@
         <v>0.5</v>
       </c>
       <c r="D22" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E22" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E22" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F22" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F22" s="38">
+        <v>2</v>
+      </c>
+      <c r="G22" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G22" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H22" s="40"/>
@@ -2961,19 +2961,19 @@
         <v>0.5</v>
       </c>
       <c r="D23" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E23" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E23" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F23" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F23" s="38">
+        <v>2</v>
+      </c>
+      <c r="G23" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G23" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H23" s="40"/>
@@ -3004,19 +3004,19 @@
         <v>0.5</v>
       </c>
       <c r="D24" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E24" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E24" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F24" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F24" s="38">
+        <v>2</v>
+      </c>
+      <c r="G24" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G24" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H24" s="40"/>
@@ -3047,19 +3047,19 @@
         <v>0.5</v>
       </c>
       <c r="D25" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E25" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E25" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F25" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F25" s="38">
+        <v>2</v>
+      </c>
+      <c r="G25" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G25" s="39">
-        <f t="shared" si="0"/>
         <v>32.002438281011884</v>
       </c>
       <c r="H25" s="40"/>
@@ -3090,19 +3090,19 @@
         <v>0.5</v>
       </c>
       <c r="D26" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E26" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E26" s="38">
+        <v>5.3337397135019806</v>
+      </c>
+      <c r="F26" s="38">
         <f t="shared" si="2"/>
-        <v>5.3337397135019806</v>
-      </c>
-      <c r="F26" s="38">
+        <v>2</v>
+      </c>
+      <c r="G26" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G26" s="39">
-        <f t="shared" si="0"/>
         <v>37.336177994513861</v>
       </c>
       <c r="H26" s="40"/>
@@ -3133,19 +3133,19 @@
         <v>0.5</v>
       </c>
       <c r="D27" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E27" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E27" s="38">
+        <v>6.0957025297165499</v>
+      </c>
+      <c r="F27" s="38">
         <f t="shared" si="2"/>
-        <v>6.0957025297165499</v>
-      </c>
-      <c r="F27" s="38">
+        <v>2</v>
+      </c>
+      <c r="G27" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G27" s="39">
-        <f t="shared" si="0"/>
         <v>42.669917708015852</v>
       </c>
       <c r="H27" s="40"/>
@@ -3176,19 +3176,19 @@
         <v>0.5</v>
       </c>
       <c r="D28" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E28" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E28" s="38">
+        <v>5.3337397135019806</v>
+      </c>
+      <c r="F28" s="38">
         <f t="shared" si="2"/>
-        <v>5.3337397135019806</v>
-      </c>
-      <c r="F28" s="38">
+        <v>2</v>
+      </c>
+      <c r="G28" s="39">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="G28" s="39">
-        <f t="shared" si="0"/>
         <v>37.336177994513861</v>
       </c>
       <c r="H28" s="40"/>
@@ -3219,19 +3219,19 @@
         <v>0.5</v>
       </c>
       <c r="D29" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E29" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E29" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F29" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F29" s="38">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G29" s="39">
         <f t="shared" si="3"/>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G29" s="39">
-        <f t="shared" si="0"/>
         <v>18.401402011581833</v>
       </c>
       <c r="H29" s="40"/>
@@ -3262,19 +3262,19 @@
         <v>0.5</v>
       </c>
       <c r="D30" s="38">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E30" s="38">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E30" s="38">
+        <v>4.5717768972874122</v>
+      </c>
+      <c r="F30" s="38">
         <f t="shared" si="2"/>
-        <v>4.5717768972874122</v>
-      </c>
-      <c r="F30" s="38">
+        <v>0.3</v>
+      </c>
+      <c r="G30" s="39">
         <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="G30" s="39">
-        <f t="shared" si="0"/>
         <v>4.800365742151782</v>
       </c>
       <c r="H30" s="40"/>
@@ -3317,7 +3317,7 @@
         <v>0.15</v>
       </c>
       <c r="G31" s="39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>11.025</v>
       </c>
       <c r="H31" s="40"/>
@@ -3476,11 +3476,11 @@
       <c r="B39" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="74">
+      <c r="C39" s="68">
         <f>J37</f>
         <v>45495.768891083135</v>
       </c>
-      <c r="D39" s="74"/>
+      <c r="D39" s="68"/>
       <c r="E39" s="51"/>
       <c r="F39" s="50"/>
       <c r="G39" s="51"/>
@@ -3494,10 +3494,10 @@
       <c r="B40" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="77">
+      <c r="C40" s="71">
         <v>40000</v>
       </c>
-      <c r="D40" s="77"/>
+      <c r="D40" s="71"/>
       <c r="E40" s="67"/>
       <c r="F40" s="48"/>
       <c r="G40" s="47"/>
@@ -3511,11 +3511,11 @@
       <c r="B41" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="78">
+      <c r="C41" s="72">
         <f>C40-C43-C44</f>
         <v>38000</v>
       </c>
-      <c r="D41" s="78"/>
+      <c r="D41" s="72"/>
       <c r="E41" s="39">
         <f>C41/C39*100</f>
         <v>83.524250553874566</v>
@@ -3532,11 +3532,11 @@
       <c r="B42" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="74">
+      <c r="C42" s="68">
         <f>C39-C41</f>
         <v>7495.7688910831348</v>
       </c>
-      <c r="D42" s="74"/>
+      <c r="D42" s="68"/>
       <c r="E42" s="39">
         <f>100-E41</f>
         <v>16.475749446125434</v>
@@ -3553,11 +3553,11 @@
       <c r="B43" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="74">
+      <c r="C43" s="68">
         <f>C40*0.03</f>
         <v>1200</v>
       </c>
-      <c r="D43" s="74"/>
+      <c r="D43" s="68"/>
       <c r="E43" s="39">
         <v>3</v>
       </c>
@@ -3573,11 +3573,11 @@
       <c r="B44" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="74">
+      <c r="C44" s="68">
         <f>C40*0.02</f>
         <v>800</v>
       </c>
-      <c r="D44" s="74"/>
+      <c r="D44" s="68"/>
       <c r="E44" s="39">
         <v>2</v>
       </c>
@@ -3652,6 +3652,13 @@
     <row r="94" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="A7:F7"/>
@@ -3660,13 +3667,6 @@
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>